<commit_message>
Version 1.6 - System backend added & Bugfixed
</commit_message>
<xml_diff>
--- a/server/data/budget.xlsx
+++ b/server/data/budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HashJGaming\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\UMLTFIPG\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F317EC-C9CC-4E8D-A310-686A65671506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDA2FF6-7137-4D13-BE4B-68ED0961DD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="0" windowWidth="23295" windowHeight="14265" xr2:uid="{A22642D4-8074-4D60-A959-8EA8FF7A55D7}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A22642D4-8074-4D60-A959-8EA8FF7A55D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Budgets</t>
-  </si>
-  <si>
     <t>PS</t>
   </si>
   <si>
@@ -64,22 +61,17 @@
   </si>
   <si>
     <t>MOOE</t>
+  </si>
+  <si>
+    <t>Project Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,7 +102,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +420,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +433,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2">
         <v>2017</v>
@@ -455,7 +447,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1181727.8</v>
@@ -469,7 +461,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>574923.4</v>
@@ -483,7 +475,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>294961.7</v>
@@ -497,7 +489,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>147480.85</v>
@@ -511,7 +503,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>147480.85</v>
@@ -525,7 +517,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>29486.17</v>
@@ -539,7 +531,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>29486.17</v>
@@ -553,7 +545,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -567,7 +559,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>544070.06000000006</v>

</xml_diff>